<commit_message>
Updated to include Reliability base implementation
</commit_message>
<xml_diff>
--- a/Data/Node_List.xlsx
+++ b/Data/Node_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11202"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoller/Box/ANCR/WAMV-Networks/multilayer_design_network_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14970A46-8C21-EA45-B283-3990ADF8A62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50982EC-B315-1B46-84B9-D87C75582CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53560" yWindow="460" windowWidth="23500" windowHeight="30380" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
+    <workbookView xWindow="38620" yWindow="460" windowWidth="28720" windowHeight="30380" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="127">
   <si>
     <t>Function</t>
   </si>
@@ -412,6 +412,9 @@
   </si>
   <si>
     <t>StartDate</t>
+  </si>
+  <si>
+    <t>Importance</t>
   </si>
 </sst>
 </file>
@@ -450,9 +453,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -769,13 +773,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A440458A-97D1-3A40-AB97-400D38B3B3DC}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D122" sqref="D122"/>
+    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -794,6 +802,9 @@
       <c r="E1" t="s">
         <v>124</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
@@ -809,6 +820,9 @@
         <v>43252</v>
       </c>
       <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2">
         <v>10</v>
       </c>
     </row>
@@ -828,6 +842,9 @@
       <c r="E3">
         <v>10</v>
       </c>
+      <c r="F3" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -845,6 +862,9 @@
       <c r="E4">
         <v>10</v>
       </c>
+      <c r="F4" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
@@ -862,6 +882,9 @@
       <c r="E5">
         <v>10</v>
       </c>
+      <c r="F5" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -879,6 +902,9 @@
       <c r="E6">
         <v>10</v>
       </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -896,6 +922,9 @@
       <c r="E7">
         <v>10</v>
       </c>
+      <c r="F7" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -913,6 +942,9 @@
       <c r="E8">
         <v>10</v>
       </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
@@ -930,6 +962,9 @@
       <c r="E9">
         <v>7.5</v>
       </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -947,6 +982,9 @@
       <c r="E10">
         <v>7.5</v>
       </c>
+      <c r="F10" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -964,6 +1002,9 @@
       <c r="E11">
         <v>7.5</v>
       </c>
+      <c r="F11" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -981,6 +1022,9 @@
       <c r="E12">
         <v>7.5</v>
       </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -998,7 +1042,9 @@
       <c r="E13">
         <v>7.5</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1016,7 +1062,9 @@
       <c r="E14">
         <v>7.5</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
@@ -1034,7 +1082,9 @@
       <c r="E15">
         <v>7.5</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -1052,7 +1102,9 @@
       <c r="E16">
         <v>7.5</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -1070,7 +1122,9 @@
       <c r="E17">
         <v>7.5</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -1088,7 +1142,9 @@
       <c r="E18">
         <v>7.5</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -1106,7 +1162,9 @@
       <c r="E19">
         <v>7.5</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="2">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -1124,7 +1182,9 @@
       <c r="E20">
         <v>7.5</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -1142,7 +1202,9 @@
       <c r="E21">
         <v>7.5</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -1160,7 +1222,9 @@
       <c r="E22">
         <v>7.5</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -1178,7 +1242,9 @@
       <c r="E23">
         <v>7.5</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -1196,7 +1262,9 @@
       <c r="E24">
         <v>7.5</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -1214,7 +1282,9 @@
       <c r="E25">
         <v>7.5</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -1232,7 +1302,9 @@
       <c r="E26">
         <v>7.5</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -1250,7 +1322,9 @@
       <c r="E27">
         <v>7.5</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -1268,7 +1342,9 @@
       <c r="E28">
         <v>7.5</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="2">
+        <v>7</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -1286,7 +1362,9 @@
       <c r="E29">
         <v>7.5</v>
       </c>
-      <c r="F29" s="1"/>
+      <c r="F29" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -1304,7 +1382,9 @@
       <c r="E30">
         <v>7.5</v>
       </c>
-      <c r="F30" s="1"/>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -1322,7 +1402,9 @@
       <c r="E31">
         <v>7.5</v>
       </c>
-      <c r="F31" s="1"/>
+      <c r="F31" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -1340,7 +1422,9 @@
       <c r="E32">
         <v>7.5</v>
       </c>
-      <c r="F32" s="1"/>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -1358,7 +1442,9 @@
       <c r="E33">
         <v>7.5</v>
       </c>
-      <c r="F33" s="1"/>
+      <c r="F33" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -1376,7 +1462,9 @@
       <c r="E34">
         <v>7.5</v>
       </c>
-      <c r="F34" s="1"/>
+      <c r="F34" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -1394,7 +1482,9 @@
       <c r="E35">
         <v>7.5</v>
       </c>
-      <c r="F35" s="1"/>
+      <c r="F35" s="2">
+        <v>6</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -1412,7 +1502,9 @@
       <c r="E36">
         <v>7.5</v>
       </c>
-      <c r="F36" s="1"/>
+      <c r="F36" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -1430,7 +1522,9 @@
       <c r="E37">
         <v>7.5</v>
       </c>
-      <c r="F37" s="1"/>
+      <c r="F37" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -1448,7 +1542,9 @@
       <c r="E38">
         <v>7.5</v>
       </c>
-      <c r="F38" s="1"/>
+      <c r="F38" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -1466,7 +1562,9 @@
       <c r="E39">
         <v>7.5</v>
       </c>
-      <c r="F39" s="1"/>
+      <c r="F39" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -1484,7 +1582,9 @@
       <c r="E40">
         <v>7.5</v>
       </c>
-      <c r="F40" s="1"/>
+      <c r="F40" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -1502,7 +1602,9 @@
       <c r="E41">
         <v>7.5</v>
       </c>
-      <c r="F41" s="1"/>
+      <c r="F41" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -1520,7 +1622,9 @@
       <c r="E42">
         <v>7.5</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -1538,7 +1642,9 @@
       <c r="E43">
         <v>7.5</v>
       </c>
-      <c r="F43" s="1"/>
+      <c r="F43" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -1556,7 +1662,9 @@
       <c r="E44">
         <v>7.5</v>
       </c>
-      <c r="F44" s="1"/>
+      <c r="F44" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -1574,7 +1682,9 @@
       <c r="E45">
         <v>7.5</v>
       </c>
-      <c r="F45" s="1"/>
+      <c r="F45" s="2">
+        <v>9</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -1592,7 +1702,9 @@
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46" s="1"/>
+      <c r="F46" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -1610,7 +1722,9 @@
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" s="1"/>
+      <c r="F47" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -1628,7 +1742,9 @@
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="1"/>
+      <c r="F48" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -1646,7 +1762,9 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49" s="1"/>
+      <c r="F49" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -1664,7 +1782,9 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" s="1"/>
+      <c r="F50" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -1682,7 +1802,9 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51" s="1"/>
+      <c r="F51" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -1700,7 +1822,9 @@
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52" s="1"/>
+      <c r="F52" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
@@ -1718,7 +1842,9 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53" s="1"/>
+      <c r="F53" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -1736,7 +1862,9 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54" s="1"/>
+      <c r="F54" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
@@ -1754,7 +1882,9 @@
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55" s="1"/>
+      <c r="F55" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -1772,7 +1902,9 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56" s="1"/>
+      <c r="F56" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -1790,7 +1922,9 @@
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57" s="1"/>
+      <c r="F57" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -1808,7 +1942,9 @@
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58" s="1"/>
+      <c r="F58" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -1826,7 +1962,9 @@
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" s="1"/>
+      <c r="F59" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -1844,7 +1982,9 @@
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60" s="1"/>
+      <c r="F60" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -1862,7 +2002,9 @@
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61" s="1"/>
+      <c r="F61" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -1880,7 +2022,9 @@
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62" s="1"/>
+      <c r="F62" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -1898,7 +2042,9 @@
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63" s="1"/>
+      <c r="F63" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -1916,7 +2062,9 @@
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64" s="1"/>
+      <c r="F64" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -1934,7 +2082,9 @@
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65" s="1"/>
+      <c r="F65" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
@@ -1952,7 +2102,9 @@
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66" s="1"/>
+      <c r="F66" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -1970,7 +2122,9 @@
       <c r="E67">
         <v>0</v>
       </c>
-      <c r="F67" s="1"/>
+      <c r="F67" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -1988,7 +2142,9 @@
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68" s="1"/>
+      <c r="F68" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -2006,7 +2162,9 @@
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69" s="1"/>
+      <c r="F69" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
@@ -2024,7 +2182,9 @@
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70" s="1"/>
+      <c r="F70" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -2042,7 +2202,9 @@
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71" s="1"/>
+      <c r="F71" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
@@ -2060,7 +2222,9 @@
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72" s="1"/>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -2078,7 +2242,9 @@
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73" s="1"/>
+      <c r="F73" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
@@ -2096,7 +2262,9 @@
       <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74" s="1"/>
+      <c r="F74" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -2114,7 +2282,9 @@
       <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75" s="1"/>
+      <c r="F75" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -2132,7 +2302,9 @@
       <c r="E76">
         <v>0</v>
       </c>
-      <c r="F76" s="1"/>
+      <c r="F76" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -2150,7 +2322,9 @@
       <c r="E77">
         <v>0</v>
       </c>
-      <c r="F77" s="1"/>
+      <c r="F77" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -2168,7 +2342,9 @@
       <c r="E78">
         <v>0</v>
       </c>
-      <c r="F78" s="1"/>
+      <c r="F78" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -2186,7 +2362,9 @@
       <c r="E79">
         <v>2.5</v>
       </c>
-      <c r="F79" s="1"/>
+      <c r="F79" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -2204,7 +2382,9 @@
       <c r="E80">
         <v>2.5</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
@@ -2222,7 +2402,9 @@
       <c r="E81">
         <v>2.5</v>
       </c>
-      <c r="F81" s="1"/>
+      <c r="F81" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -2240,7 +2422,9 @@
       <c r="E82">
         <v>2.5</v>
       </c>
-      <c r="F82" s="1"/>
+      <c r="F82" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
@@ -2258,7 +2442,9 @@
       <c r="E83">
         <v>2.5</v>
       </c>
-      <c r="F83" s="1"/>
+      <c r="F83" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -2276,7 +2462,9 @@
       <c r="E84">
         <v>2.5</v>
       </c>
-      <c r="F84" s="1"/>
+      <c r="F84" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -2294,7 +2482,9 @@
       <c r="E85">
         <v>2.5</v>
       </c>
-      <c r="F85" s="1"/>
+      <c r="F85" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -2312,7 +2502,9 @@
       <c r="E86">
         <v>2.5</v>
       </c>
-      <c r="F86" s="1"/>
+      <c r="F86" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -2330,7 +2522,9 @@
       <c r="E87">
         <v>2.5</v>
       </c>
-      <c r="F87" s="1"/>
+      <c r="F87" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
@@ -2348,7 +2542,9 @@
       <c r="E88">
         <v>2.5</v>
       </c>
-      <c r="F88" s="1"/>
+      <c r="F88" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
@@ -2366,7 +2562,9 @@
       <c r="E89">
         <v>2.5</v>
       </c>
-      <c r="F89" s="1"/>
+      <c r="F89" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -2384,7 +2582,9 @@
       <c r="E90">
         <v>2.5</v>
       </c>
-      <c r="F90" s="1"/>
+      <c r="F90" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
@@ -2402,7 +2602,9 @@
       <c r="E91">
         <v>2.5</v>
       </c>
-      <c r="F91" s="1"/>
+      <c r="F91" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
@@ -2420,7 +2622,9 @@
       <c r="E92">
         <v>2.5</v>
       </c>
-      <c r="F92" s="1"/>
+      <c r="F92" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
@@ -2438,7 +2642,9 @@
       <c r="E93">
         <v>2.5</v>
       </c>
-      <c r="F93" s="1"/>
+      <c r="F93" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
@@ -2456,7 +2662,9 @@
       <c r="E94">
         <v>2.5</v>
       </c>
-      <c r="F94" s="1"/>
+      <c r="F94" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
@@ -2474,7 +2682,9 @@
       <c r="E95">
         <v>2.5</v>
       </c>
-      <c r="F95" s="1"/>
+      <c r="F95" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
@@ -2492,7 +2702,9 @@
       <c r="E96">
         <v>10</v>
       </c>
-      <c r="F96" s="1"/>
+      <c r="F96" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
@@ -2510,7 +2722,9 @@
       <c r="E97">
         <v>0</v>
       </c>
-      <c r="F97" s="1"/>
+      <c r="F97" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
@@ -2528,7 +2742,9 @@
       <c r="E98">
         <v>0</v>
       </c>
-      <c r="F98" s="1"/>
+      <c r="F98" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
@@ -2546,7 +2762,9 @@
       <c r="E99">
         <v>0</v>
       </c>
-      <c r="F99" s="1"/>
+      <c r="F99" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
@@ -2564,7 +2782,9 @@
       <c r="E100">
         <v>0</v>
       </c>
-      <c r="F100" s="1"/>
+      <c r="F100" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
@@ -2582,7 +2802,9 @@
       <c r="E101">
         <v>0</v>
       </c>
-      <c r="F101" s="1"/>
+      <c r="F101" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
@@ -2600,7 +2822,9 @@
       <c r="E102">
         <v>0</v>
       </c>
-      <c r="F102" s="1"/>
+      <c r="F102" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
@@ -2618,7 +2842,9 @@
       <c r="E103">
         <v>0</v>
       </c>
-      <c r="F103" s="1"/>
+      <c r="F103" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
@@ -2636,6 +2862,9 @@
       <c r="E104">
         <v>5</v>
       </c>
+      <c r="F104" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
@@ -2653,6 +2882,9 @@
       <c r="E105">
         <v>5</v>
       </c>
+      <c r="F105" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
@@ -2670,6 +2902,9 @@
       <c r="E106">
         <v>5</v>
       </c>
+      <c r="F106" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
@@ -2687,6 +2922,9 @@
       <c r="E107">
         <v>5</v>
       </c>
+      <c r="F107" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
@@ -2704,6 +2942,9 @@
       <c r="E108">
         <v>5</v>
       </c>
+      <c r="F108" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
@@ -2721,6 +2962,9 @@
       <c r="E109">
         <v>5</v>
       </c>
+      <c r="F109" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
@@ -2738,6 +2982,9 @@
       <c r="E110">
         <v>5</v>
       </c>
+      <c r="F110" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
@@ -2755,6 +3002,9 @@
       <c r="E111">
         <v>5</v>
       </c>
+      <c r="F111" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
@@ -2772,8 +3022,11 @@
       <c r="E112">
         <v>5</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F112" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2789,8 +3042,11 @@
       <c r="E113">
         <v>5</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F113" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2806,8 +3062,11 @@
       <c r="E114">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F114" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2823,8 +3082,11 @@
       <c r="E115">
         <v>5</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F115" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2840,8 +3102,11 @@
       <c r="E116">
         <v>5</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F116" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2857,8 +3122,11 @@
       <c r="E117">
         <v>5</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F117" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2874,8 +3142,11 @@
       <c r="E118">
         <v>5</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F118" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2891,8 +3162,11 @@
       <c r="E119">
         <v>5</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F119" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2908,8 +3182,11 @@
       <c r="E120">
         <v>5</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F120" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2924,6 +3201,9 @@
       </c>
       <c r="E121">
         <v>5</v>
+      </c>
+      <c r="F121" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created a new create graph function to add node attributes
</commit_message>
<xml_diff>
--- a/Data/Node_List.xlsx
+++ b/Data/Node_List.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoller/Box/ANCR/WAMV-Networks/multilayer_design_network_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50982EC-B315-1B46-84B9-D87C75582CAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{58865051-2F88-F34A-BC89-E74EADF9E0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38620" yWindow="460" windowWidth="28720" windowHeight="30380" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
+    <workbookView xWindow="1480" yWindow="2500" windowWidth="28720" windowHeight="14400" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Nodes" sheetId="1" r:id="rId1"/>
-    <sheet name="Lookup" sheetId="2" r:id="rId2"/>
+    <sheet name="Node_List" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -773,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A440458A-97D1-3A40-AB97-400D38B3B3DC}">
   <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3210,18 +3209,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4DE0F0-F6DD-964E-911D-B2EF69A8D7FA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added time series capability and data creation
</commit_message>
<xml_diff>
--- a/Data/Node_List.xlsx
+++ b/Data/Node_List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jcoller/Box/ANCR/WAMV-Networks/multilayer_design_network_tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58865051-2F88-F34A-BC89-E74EADF9E0B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C033D40A-FF0B-0140-9498-345A69F03726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="2500" windowWidth="28720" windowHeight="14400" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
+    <workbookView xWindow="16200" yWindow="2820" windowWidth="28720" windowHeight="14400" xr2:uid="{320C58FC-2FC4-CE4C-8486-5CFAF2D324D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Node_List" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -454,8 +454,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,16 +773,16 @@
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -795,13 +795,13 @@
       <c r="C1" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>125</v>
       </c>
       <c r="E1" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>126</v>
       </c>
     </row>
@@ -815,13 +815,13 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>43252</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>10</v>
       </c>
     </row>
@@ -835,13 +835,13 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>43331</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>7</v>
       </c>
     </row>
@@ -855,13 +855,13 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <v>43151</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>3</v>
       </c>
     </row>
@@ -875,13 +875,13 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>43392</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>5</v>
       </c>
     </row>
@@ -895,13 +895,13 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>43423</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
     </row>
@@ -915,13 +915,13 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>43423</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>5</v>
       </c>
     </row>
@@ -935,13 +935,13 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>43270</v>
       </c>
       <c r="E8">
         <v>10</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>10</v>
       </c>
     </row>
@@ -955,13 +955,13 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>43270</v>
       </c>
       <c r="E9">
         <v>7.5</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>10</v>
       </c>
     </row>
@@ -975,13 +975,13 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>43270</v>
       </c>
       <c r="E10">
         <v>7.5</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>10</v>
       </c>
     </row>
@@ -995,13 +995,13 @@
       <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>43239</v>
       </c>
       <c r="E11">
         <v>7.5</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1015,13 +1015,13 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>43239</v>
       </c>
       <c r="E12">
         <v>7.5</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1035,13 +1035,13 @@
       <c r="C13" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>43300</v>
       </c>
       <c r="E13">
         <v>7.5</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1055,13 +1055,13 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>43239</v>
       </c>
       <c r="E14">
         <v>7.5</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1075,13 +1075,13 @@
       <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>43239</v>
       </c>
       <c r="E15">
         <v>7.5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1095,13 +1095,13 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>43270</v>
       </c>
       <c r="E16">
         <v>7.5</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1115,13 +1115,13 @@
       <c r="C17" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>43270</v>
       </c>
       <c r="E17">
         <v>7.5</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1135,13 +1135,13 @@
       <c r="C18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>43239</v>
       </c>
       <c r="E18">
         <v>7.5</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1155,13 +1155,13 @@
       <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>43239</v>
       </c>
       <c r="E19">
         <v>7.5</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>8</v>
       </c>
     </row>
@@ -1175,13 +1175,13 @@
       <c r="C20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <v>43331</v>
       </c>
       <c r="E20">
         <v>7.5</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1195,13 +1195,13 @@
       <c r="C21" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>43392</v>
       </c>
       <c r="E21">
         <v>7.5</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1215,13 +1215,13 @@
       <c r="C22" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>43331</v>
       </c>
       <c r="E22">
         <v>7.5</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1235,13 +1235,13 @@
       <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <v>43331</v>
       </c>
       <c r="E23">
         <v>7.5</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1255,13 +1255,13 @@
       <c r="C24" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="2">
         <v>43331</v>
       </c>
       <c r="E24">
         <v>7.5</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1275,13 +1275,13 @@
       <c r="C25" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <v>43300</v>
       </c>
       <c r="E25">
         <v>7.5</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1295,13 +1295,13 @@
       <c r="C26" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <v>43300</v>
       </c>
       <c r="E26">
         <v>7.5</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1315,13 +1315,13 @@
       <c r="C27" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2">
         <v>43300</v>
       </c>
       <c r="E27">
         <v>7.5</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1335,13 +1335,13 @@
       <c r="C28" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="2">
         <v>43300</v>
       </c>
       <c r="E28">
         <v>7.5</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>7</v>
       </c>
     </row>
@@ -1355,13 +1355,13 @@
       <c r="C29" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>43392</v>
       </c>
       <c r="E29">
         <v>7.5</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1375,13 +1375,13 @@
       <c r="C30" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <v>43423</v>
       </c>
       <c r="E30">
         <v>7.5</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1395,13 +1395,13 @@
       <c r="C31" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="2">
         <v>43362</v>
       </c>
       <c r="E31">
         <v>7.5</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1415,13 +1415,13 @@
       <c r="C32" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="2">
         <v>43331</v>
       </c>
       <c r="E32">
         <v>7.5</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1435,13 +1435,13 @@
       <c r="C33" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="2">
         <v>43392</v>
       </c>
       <c r="E33">
         <v>7.5</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1455,13 +1455,13 @@
       <c r="C34" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="2">
         <v>43392</v>
       </c>
       <c r="E34">
         <v>7.5</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>5</v>
       </c>
     </row>
@@ -1475,13 +1475,13 @@
       <c r="C35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <v>43300</v>
       </c>
       <c r="E35">
         <v>7.5</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>6</v>
       </c>
     </row>
@@ -1495,13 +1495,13 @@
       <c r="C36" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <v>43423</v>
       </c>
       <c r="E36">
         <v>7.5</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1515,13 +1515,13 @@
       <c r="C37" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <v>43423</v>
       </c>
       <c r="E37">
         <v>7.5</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1535,13 +1535,13 @@
       <c r="C38" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <v>43423</v>
       </c>
       <c r="E38">
         <v>7.5</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>3</v>
       </c>
     </row>
@@ -1555,13 +1555,13 @@
       <c r="C39" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <v>43362</v>
       </c>
       <c r="E39">
         <v>7.5</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1575,13 +1575,13 @@
       <c r="C40" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <v>43392</v>
       </c>
       <c r="E40">
         <v>7.5</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>2</v>
       </c>
     </row>
@@ -1595,13 +1595,13 @@
       <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="2">
         <v>43270</v>
       </c>
       <c r="E41">
         <v>7.5</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1615,13 +1615,13 @@
       <c r="C42" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <v>43270</v>
       </c>
       <c r="E42">
         <v>7.5</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1635,13 +1635,13 @@
       <c r="C43" t="s">
         <v>42</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="2">
         <v>43270</v>
       </c>
       <c r="E43">
         <v>7.5</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1655,13 +1655,13 @@
       <c r="C44" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="2">
         <v>43270</v>
       </c>
       <c r="E44">
         <v>7.5</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1675,13 +1675,13 @@
       <c r="C45" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="2">
         <v>43270</v>
       </c>
       <c r="E45">
         <v>7.5</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1695,13 +1695,13 @@
       <c r="C46" t="s">
         <v>47</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <v>43191</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1715,13 +1715,13 @@
       <c r="C47" t="s">
         <v>48</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <v>43191</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1735,13 +1735,13 @@
       <c r="C48" t="s">
         <v>49</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>43221</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1755,13 +1755,13 @@
       <c r="C49" t="s">
         <v>50</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="2">
         <v>43435</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1775,13 +1775,13 @@
       <c r="C50" t="s">
         <v>51</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="2">
         <v>43221</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1795,13 +1795,13 @@
       <c r="C51" t="s">
         <v>52</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="2">
         <v>43435</v>
       </c>
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1815,13 +1815,13 @@
       <c r="C52" t="s">
         <v>53</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="2">
         <v>43252</v>
       </c>
       <c r="E52">
         <v>0</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1835,13 +1835,13 @@
       <c r="C53" t="s">
         <v>54</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="2">
         <v>43252</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1855,13 +1855,13 @@
       <c r="C54" t="s">
         <v>55</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="2">
         <v>43344</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1875,13 +1875,13 @@
       <c r="C55" t="s">
         <v>56</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="2">
         <v>43344</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1895,13 +1895,13 @@
       <c r="C56" t="s">
         <v>57</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="2">
         <v>43252</v>
       </c>
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1915,13 +1915,13 @@
       <c r="C57" t="s">
         <v>58</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="2">
         <v>43252</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1935,13 +1935,13 @@
       <c r="C58" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="2">
         <v>43282</v>
       </c>
       <c r="E58">
         <v>0</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1955,13 +1955,13 @@
       <c r="C59" t="s">
         <v>60</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="2">
         <v>43282</v>
       </c>
       <c r="E59">
         <v>0</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1975,13 +1975,13 @@
       <c r="C60" t="s">
         <v>61</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="2">
         <v>43282</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="1">
         <v>0</v>
       </c>
     </row>
@@ -1995,13 +1995,13 @@
       <c r="C61" t="s">
         <v>62</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="2">
         <v>43282</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2015,13 +2015,13 @@
       <c r="C62" t="s">
         <v>63</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="2">
         <v>43282</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2035,13 +2035,13 @@
       <c r="C63" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="2">
         <v>43282</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2055,13 +2055,13 @@
       <c r="C64" t="s">
         <v>65</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="2">
         <v>43344</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2075,13 +2075,13 @@
       <c r="C65" t="s">
         <v>66</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="2">
         <v>43252</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2095,13 +2095,13 @@
       <c r="C66" t="s">
         <v>67</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="2">
         <v>43252</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2115,13 +2115,13 @@
       <c r="C67" t="s">
         <v>68</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="2">
         <v>43252</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2135,13 +2135,13 @@
       <c r="C68" t="s">
         <v>69</v>
       </c>
-      <c r="D68" s="1">
+      <c r="D68" s="2">
         <v>43252</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2155,13 +2155,13 @@
       <c r="C69" t="s">
         <v>70</v>
       </c>
-      <c r="D69" s="1">
+      <c r="D69" s="2">
         <v>43252</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2175,13 +2175,13 @@
       <c r="C70" t="s">
         <v>71</v>
       </c>
-      <c r="D70" s="1">
+      <c r="D70" s="2">
         <v>43282</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
-      <c r="F70" s="2">
+      <c r="F70" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2195,13 +2195,13 @@
       <c r="C71" t="s">
         <v>72</v>
       </c>
-      <c r="D71" s="1">
+      <c r="D71" s="2">
         <v>43282</v>
       </c>
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2215,13 +2215,13 @@
       <c r="C72" t="s">
         <v>73</v>
       </c>
-      <c r="D72" s="1">
+      <c r="D72" s="2">
         <v>43221</v>
       </c>
       <c r="E72">
         <v>0</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2235,13 +2235,13 @@
       <c r="C73" t="s">
         <v>74</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="2">
         <v>43221</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2255,13 +2255,13 @@
       <c r="C74" t="s">
         <v>75</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="2">
         <v>43221</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2275,13 +2275,13 @@
       <c r="C75" t="s">
         <v>77</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="2">
         <v>43221</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2295,13 +2295,13 @@
       <c r="C76" t="s">
         <v>76</v>
       </c>
-      <c r="D76" s="1">
+      <c r="D76" s="2">
         <v>43221</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2315,13 +2315,13 @@
       <c r="C77" t="s">
         <v>78</v>
       </c>
-      <c r="D77" s="1">
+      <c r="D77" s="2">
         <v>43221</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2335,13 +2335,13 @@
       <c r="C78" t="s">
         <v>82</v>
       </c>
-      <c r="D78" s="1">
+      <c r="D78" s="2">
         <v>43405</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2355,13 +2355,13 @@
       <c r="C79" t="s">
         <v>83</v>
       </c>
-      <c r="D79" s="1">
+      <c r="D79" s="2">
         <v>43209</v>
       </c>
       <c r="E79">
         <v>2.5</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2375,13 +2375,13 @@
       <c r="C80" t="s">
         <v>84</v>
       </c>
-      <c r="D80" s="1">
+      <c r="D80" s="2">
         <v>43300</v>
       </c>
       <c r="E80">
         <v>2.5</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2395,13 +2395,13 @@
       <c r="C81" t="s">
         <v>85</v>
       </c>
-      <c r="D81" s="1">
+      <c r="D81" s="2">
         <v>43300</v>
       </c>
       <c r="E81">
         <v>2.5</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2415,13 +2415,13 @@
       <c r="C82" t="s">
         <v>86</v>
       </c>
-      <c r="D82" s="1">
+      <c r="D82" s="2">
         <v>43270</v>
       </c>
       <c r="E82">
         <v>2.5</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2435,13 +2435,13 @@
       <c r="C83" t="s">
         <v>24</v>
       </c>
-      <c r="D83" s="1">
+      <c r="D83" s="2">
         <v>43300</v>
       </c>
       <c r="E83">
         <v>2.5</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2455,13 +2455,13 @@
       <c r="C84" t="s">
         <v>87</v>
       </c>
-      <c r="D84" s="1">
+      <c r="D84" s="2">
         <v>43362</v>
       </c>
       <c r="E84">
         <v>2.5</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2475,13 +2475,13 @@
       <c r="C85" t="s">
         <v>88</v>
       </c>
-      <c r="D85" s="1">
+      <c r="D85" s="2">
         <v>43300</v>
       </c>
       <c r="E85">
         <v>2.5</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2495,13 +2495,13 @@
       <c r="C86" t="s">
         <v>89</v>
       </c>
-      <c r="D86" s="1">
+      <c r="D86" s="2">
         <v>43331</v>
       </c>
       <c r="E86">
         <v>2.5</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2515,13 +2515,13 @@
       <c r="C87" t="s">
         <v>90</v>
       </c>
-      <c r="D87" s="1">
+      <c r="D87" s="2">
         <v>43331</v>
       </c>
       <c r="E87">
         <v>2.5</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2535,13 +2535,13 @@
       <c r="C88" t="s">
         <v>21</v>
       </c>
-      <c r="D88" s="1">
+      <c r="D88" s="2">
         <v>43300</v>
       </c>
       <c r="E88">
         <v>2.5</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2555,13 +2555,13 @@
       <c r="C89" t="s">
         <v>22</v>
       </c>
-      <c r="D89" s="1">
+      <c r="D89" s="2">
         <v>43362</v>
       </c>
       <c r="E89">
         <v>2.5</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2575,13 +2575,13 @@
       <c r="C90" t="s">
         <v>91</v>
       </c>
-      <c r="D90" s="1">
+      <c r="D90" s="2">
         <v>43270</v>
       </c>
       <c r="E90">
         <v>2.5</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2595,13 +2595,13 @@
       <c r="C91" t="s">
         <v>92</v>
       </c>
-      <c r="D91" s="1">
+      <c r="D91" s="2">
         <v>43300</v>
       </c>
       <c r="E91">
         <v>2.5</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2615,13 +2615,13 @@
       <c r="C92" t="s">
         <v>93</v>
       </c>
-      <c r="D92" s="1">
+      <c r="D92" s="2">
         <v>43300</v>
       </c>
       <c r="E92">
         <v>2.5</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2635,13 +2635,13 @@
       <c r="C93" t="s">
         <v>94</v>
       </c>
-      <c r="D93" s="1">
+      <c r="D93" s="2">
         <v>43239</v>
       </c>
       <c r="E93">
         <v>2.5</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2655,13 +2655,13 @@
       <c r="C94" t="s">
         <v>95</v>
       </c>
-      <c r="D94" s="1">
+      <c r="D94" s="2">
         <v>43239</v>
       </c>
       <c r="E94">
         <v>2.5</v>
       </c>
-      <c r="F94" s="2">
+      <c r="F94" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2675,13 +2675,13 @@
       <c r="C95" t="s">
         <v>96</v>
       </c>
-      <c r="D95" s="1">
+      <c r="D95" s="2">
         <v>43423</v>
       </c>
       <c r="E95">
         <v>2.5</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2695,13 +2695,13 @@
       <c r="C96" t="s">
         <v>98</v>
       </c>
-      <c r="D96" s="1">
+      <c r="D96" s="2">
         <v>43435</v>
       </c>
       <c r="E96">
         <v>10</v>
       </c>
-      <c r="F96" s="2">
+      <c r="F96" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2715,13 +2715,13 @@
       <c r="C97" t="s">
         <v>99</v>
       </c>
-      <c r="D97" s="1">
+      <c r="D97" s="2">
         <v>43252</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2735,13 +2735,13 @@
       <c r="C98" t="s">
         <v>100</v>
       </c>
-      <c r="D98" s="1">
+      <c r="D98" s="2">
         <v>43252</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2755,13 +2755,13 @@
       <c r="C99" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="1">
+      <c r="D99" s="2">
         <v>43252</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
-      <c r="F99" s="2">
+      <c r="F99" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2775,13 +2775,13 @@
       <c r="C100" t="s">
         <v>102</v>
       </c>
-      <c r="D100" s="1">
+      <c r="D100" s="2">
         <v>43344</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
-      <c r="F100" s="2">
+      <c r="F100" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2795,13 +2795,13 @@
       <c r="C101" t="s">
         <v>103</v>
       </c>
-      <c r="D101" s="1">
+      <c r="D101" s="2">
         <v>43252</v>
       </c>
       <c r="E101">
         <v>0</v>
       </c>
-      <c r="F101" s="2">
+      <c r="F101" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2815,13 +2815,13 @@
       <c r="C102" t="s">
         <v>104</v>
       </c>
-      <c r="D102" s="1">
+      <c r="D102" s="2">
         <v>43252</v>
       </c>
       <c r="E102">
         <v>0</v>
       </c>
-      <c r="F102" s="2">
+      <c r="F102" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2835,13 +2835,13 @@
       <c r="C103" t="s">
         <v>105</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="2">
         <v>43252</v>
       </c>
       <c r="E103">
         <v>0</v>
       </c>
-      <c r="F103" s="2">
+      <c r="F103" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2855,13 +2855,13 @@
       <c r="C104" t="s">
         <v>107</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="2">
         <v>43282</v>
       </c>
       <c r="E104">
         <v>5</v>
       </c>
-      <c r="F104" s="2">
+      <c r="F104" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2875,13 +2875,13 @@
       <c r="C105" t="s">
         <v>108</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="2">
         <v>43282</v>
       </c>
       <c r="E105">
         <v>5</v>
       </c>
-      <c r="F105" s="2">
+      <c r="F105" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2895,13 +2895,13 @@
       <c r="C106" t="s">
         <v>109</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="2">
         <v>43282</v>
       </c>
       <c r="E106">
         <v>5</v>
       </c>
-      <c r="F106" s="2">
+      <c r="F106" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2915,13 +2915,13 @@
       <c r="C107" t="s">
         <v>21</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="2">
         <v>43282</v>
       </c>
       <c r="E107">
         <v>5</v>
       </c>
-      <c r="F107" s="2">
+      <c r="F107" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2935,13 +2935,13 @@
       <c r="C108" t="s">
         <v>110</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="2">
         <v>43282</v>
       </c>
       <c r="E108">
         <v>5</v>
       </c>
-      <c r="F108" s="2">
+      <c r="F108" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2955,13 +2955,13 @@
       <c r="C109" t="s">
         <v>111</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="2">
         <v>43282</v>
       </c>
       <c r="E109">
         <v>5</v>
       </c>
-      <c r="F109" s="2">
+      <c r="F109" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2975,13 +2975,13 @@
       <c r="C110" t="s">
         <v>112</v>
       </c>
-      <c r="D110" s="1">
+      <c r="D110" s="2">
         <v>43282</v>
       </c>
       <c r="E110">
         <v>5</v>
       </c>
-      <c r="F110" s="2">
+      <c r="F110" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2995,13 +2995,13 @@
       <c r="C111" t="s">
         <v>113</v>
       </c>
-      <c r="D111" s="1">
+      <c r="D111" s="2">
         <v>43282</v>
       </c>
       <c r="E111">
         <v>5</v>
       </c>
-      <c r="F111" s="2">
+      <c r="F111" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3015,13 +3015,13 @@
       <c r="C112" t="s">
         <v>114</v>
       </c>
-      <c r="D112" s="1">
+      <c r="D112" s="2">
         <v>43282</v>
       </c>
       <c r="E112">
         <v>5</v>
       </c>
-      <c r="F112" s="2">
+      <c r="F112" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3035,13 +3035,13 @@
       <c r="C113" t="s">
         <v>115</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="2">
         <v>43282</v>
       </c>
       <c r="E113">
         <v>5</v>
       </c>
-      <c r="F113" s="2">
+      <c r="F113" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3055,13 +3055,13 @@
       <c r="C114" t="s">
         <v>116</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="2">
         <v>43282</v>
       </c>
       <c r="E114">
         <v>5</v>
       </c>
-      <c r="F114" s="2">
+      <c r="F114" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3075,13 +3075,13 @@
       <c r="C115" t="s">
         <v>117</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="2">
         <v>43282</v>
       </c>
       <c r="E115">
         <v>5</v>
       </c>
-      <c r="F115" s="2">
+      <c r="F115" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3095,13 +3095,13 @@
       <c r="C116" t="s">
         <v>118</v>
       </c>
-      <c r="D116" s="1">
+      <c r="D116" s="2">
         <v>43282</v>
       </c>
       <c r="E116">
         <v>5</v>
       </c>
-      <c r="F116" s="2">
+      <c r="F116" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3115,13 +3115,13 @@
       <c r="C117" t="s">
         <v>119</v>
       </c>
-      <c r="D117" s="1">
+      <c r="D117" s="2">
         <v>43282</v>
       </c>
       <c r="E117">
         <v>5</v>
       </c>
-      <c r="F117" s="2">
+      <c r="F117" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3135,13 +3135,13 @@
       <c r="C118" t="s">
         <v>120</v>
       </c>
-      <c r="D118" s="1">
+      <c r="D118" s="2">
         <v>43282</v>
       </c>
       <c r="E118">
         <v>5</v>
       </c>
-      <c r="F118" s="2">
+      <c r="F118" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3155,13 +3155,13 @@
       <c r="C119" t="s">
         <v>121</v>
       </c>
-      <c r="D119" s="1">
+      <c r="D119" s="2">
         <v>43282</v>
       </c>
       <c r="E119">
         <v>5</v>
       </c>
-      <c r="F119" s="2">
+      <c r="F119" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3175,13 +3175,13 @@
       <c r="C120" t="s">
         <v>122</v>
       </c>
-      <c r="D120" s="1">
+      <c r="D120" s="2">
         <v>43282</v>
       </c>
       <c r="E120">
         <v>5</v>
       </c>
-      <c r="F120" s="2">
+      <c r="F120" s="1">
         <v>0</v>
       </c>
     </row>
@@ -3195,13 +3195,13 @@
       <c r="C121" t="s">
         <v>123</v>
       </c>
-      <c r="D121" s="1">
+      <c r="D121" s="2">
         <v>43282</v>
       </c>
       <c r="E121">
         <v>5</v>
       </c>
-      <c r="F121" s="2">
+      <c r="F121" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>